<commit_message>
change to afwerking in test door XDOVCL-2053
</commit_message>
<xml_diff>
--- a/tests/data/filled_templates/grondwater_template_full2.xlsx
+++ b/tests/data/filled_templates/grondwater_template_full2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RubenVijverman\PycharmProjects\xls2xml\tests\data\filled_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0153A2-3B79-41E0-A1F2-F3879875B3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA04C5E8-F4AC-4AB2-B1D9-44B59846106D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codelijsten" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10424" uniqueCount="3208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10424" uniqueCount="3209">
   <si>
     <t>identificatie</t>
   </si>
@@ -9650,6 +9650,9 @@
   </si>
   <si>
     <t>Noendries</t>
+  </si>
+  <si>
+    <t>afwerking-materiaal</t>
   </si>
 </sst>
 </file>
@@ -39673,11 +39676,70 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="EY2:EZ2"/>
-    <mergeCell ref="FA2:FB2"/>
-    <mergeCell ref="EU1:FB1"/>
-    <mergeCell ref="FC2:FD2"/>
-    <mergeCell ref="FC1:FD1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="A1:AL1"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="AY2:AZ2"/>
+    <mergeCell ref="BA2:BB2"/>
+    <mergeCell ref="BC2:BD2"/>
+    <mergeCell ref="BE2:BF2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="CA2:CB2"/>
+    <mergeCell ref="CC2:CD2"/>
+    <mergeCell ref="CE2:CF2"/>
+    <mergeCell ref="AM1:CF1"/>
+    <mergeCell ref="CG2:CH2"/>
+    <mergeCell ref="BQ2:BR2"/>
+    <mergeCell ref="BS2:BT2"/>
+    <mergeCell ref="BU2:BV2"/>
+    <mergeCell ref="BW2:BX2"/>
+    <mergeCell ref="BY2:BZ2"/>
+    <mergeCell ref="BG2:BH2"/>
+    <mergeCell ref="BI2:BJ2"/>
+    <mergeCell ref="BK2:BL2"/>
+    <mergeCell ref="BM2:BN2"/>
+    <mergeCell ref="BO2:BP2"/>
+    <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="CI2:CJ2"/>
+    <mergeCell ref="CK2:CL2"/>
+    <mergeCell ref="CM2:CN2"/>
+    <mergeCell ref="CO2:CP2"/>
+    <mergeCell ref="CQ2:CR2"/>
+    <mergeCell ref="CS2:CT2"/>
+    <mergeCell ref="CU2:CV2"/>
+    <mergeCell ref="CW2:CX2"/>
+    <mergeCell ref="CY2:CZ2"/>
+    <mergeCell ref="DA2:DB2"/>
+    <mergeCell ref="DO2:DP2"/>
+    <mergeCell ref="DQ2:DR2"/>
+    <mergeCell ref="DS2:DT2"/>
+    <mergeCell ref="DU2:DV2"/>
+    <mergeCell ref="DC2:DD2"/>
+    <mergeCell ref="DE2:DF2"/>
+    <mergeCell ref="DG2:DH2"/>
+    <mergeCell ref="DI2:DJ2"/>
+    <mergeCell ref="DK2:DL2"/>
     <mergeCell ref="EQ2:ER2"/>
     <mergeCell ref="ES2:ET2"/>
     <mergeCell ref="CG1:ET1"/>
@@ -39694,70 +39756,11 @@
     <mergeCell ref="EC2:ED2"/>
     <mergeCell ref="EE2:EF2"/>
     <mergeCell ref="DM2:DN2"/>
-    <mergeCell ref="DO2:DP2"/>
-    <mergeCell ref="DQ2:DR2"/>
-    <mergeCell ref="DS2:DT2"/>
-    <mergeCell ref="DU2:DV2"/>
-    <mergeCell ref="DC2:DD2"/>
-    <mergeCell ref="DE2:DF2"/>
-    <mergeCell ref="DG2:DH2"/>
-    <mergeCell ref="DI2:DJ2"/>
-    <mergeCell ref="DK2:DL2"/>
-    <mergeCell ref="CS2:CT2"/>
-    <mergeCell ref="CU2:CV2"/>
-    <mergeCell ref="CW2:CX2"/>
-    <mergeCell ref="CY2:CZ2"/>
-    <mergeCell ref="DA2:DB2"/>
-    <mergeCell ref="CI2:CJ2"/>
-    <mergeCell ref="CK2:CL2"/>
-    <mergeCell ref="CM2:CN2"/>
-    <mergeCell ref="CO2:CP2"/>
-    <mergeCell ref="CQ2:CR2"/>
-    <mergeCell ref="CA2:CB2"/>
-    <mergeCell ref="CC2:CD2"/>
-    <mergeCell ref="CE2:CF2"/>
-    <mergeCell ref="AM1:CF1"/>
-    <mergeCell ref="CG2:CH2"/>
-    <mergeCell ref="BQ2:BR2"/>
-    <mergeCell ref="BS2:BT2"/>
-    <mergeCell ref="BU2:BV2"/>
-    <mergeCell ref="BW2:BX2"/>
-    <mergeCell ref="BY2:BZ2"/>
-    <mergeCell ref="BG2:BH2"/>
-    <mergeCell ref="BI2:BJ2"/>
-    <mergeCell ref="BK2:BL2"/>
-    <mergeCell ref="BM2:BN2"/>
-    <mergeCell ref="BO2:BP2"/>
-    <mergeCell ref="AW2:AX2"/>
-    <mergeCell ref="AY2:AZ2"/>
-    <mergeCell ref="BA2:BB2"/>
-    <mergeCell ref="BC2:BD2"/>
-    <mergeCell ref="BE2:BF2"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AQ2:AR2"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="A1:AL1"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="EY2:EZ2"/>
+    <mergeCell ref="FA2:FB2"/>
+    <mergeCell ref="EU1:FB1"/>
+    <mergeCell ref="FC2:FD2"/>
+    <mergeCell ref="FC1:FD1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="80">
@@ -39849,8 +39852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:DB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CN7" workbookViewId="0">
-      <selection activeCell="CQ15" sqref="CQ15"/>
+    <sheetView tabSelected="1" topLeftCell="BU1" workbookViewId="0">
+      <selection activeCell="BW16" sqref="BW16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39956,7 +39959,7 @@
     <col min="106" max="106" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:106" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -40183,7 +40186,7 @@
         <v>108</v>
       </c>
       <c r="BX1" s="1" t="s">
-        <v>110</v>
+        <v>3208</v>
       </c>
       <c r="BY1" s="1" t="s">
         <v>113</v>
@@ -40276,7 +40279,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:106" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:106" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -40420,7 +40423,7 @@
       <c r="DA2" s="8"/>
       <c r="DB2" s="8"/>
     </row>
-    <row r="3" spans="1:106" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:106" x14ac:dyDescent="0.3">
       <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
@@ -40577,7 +40580,7 @@
       </c>
       <c r="DB3" s="8"/>
     </row>
-    <row r="4" spans="1:106" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:106" x14ac:dyDescent="0.3">
       <c r="I4" s="6" t="s">
         <v>12</v>
       </c>
@@ -40750,7 +40753,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:106" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:106" x14ac:dyDescent="0.3">
       <c r="M5" s="6" t="s">
         <v>20</v>
       </c>
@@ -40829,7 +40832,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:106" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:106" x14ac:dyDescent="0.3">
       <c r="N6" s="6" t="s">
         <v>22</v>
       </c>
@@ -41379,6 +41382,29 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="M4:T4"/>
+    <mergeCell ref="I3:T3"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AG5"/>
+    <mergeCell ref="Z4:AG4"/>
+    <mergeCell ref="W3:AH3"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AO5:AS5"/>
+    <mergeCell ref="AL4:AS4"/>
+    <mergeCell ref="AI3:AT3"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="BA5:BE5"/>
+    <mergeCell ref="AX4:BE4"/>
+    <mergeCell ref="AU3:BF3"/>
+    <mergeCell ref="BG3:BH3"/>
+    <mergeCell ref="I2:BH2"/>
+    <mergeCell ref="BN4:BO4"/>
+    <mergeCell ref="BP4:BT4"/>
+    <mergeCell ref="BM3:BT3"/>
+    <mergeCell ref="BL2:BU2"/>
     <mergeCell ref="DA3:DB3"/>
     <mergeCell ref="CT2:DB2"/>
     <mergeCell ref="BV2:CH2"/>
@@ -41391,29 +41417,6 @@
     <mergeCell ref="CC3:CD3"/>
     <mergeCell ref="CE3:CF3"/>
     <mergeCell ref="CG3:CH3"/>
-    <mergeCell ref="BG3:BH3"/>
-    <mergeCell ref="I2:BH2"/>
-    <mergeCell ref="BN4:BO4"/>
-    <mergeCell ref="BP4:BT4"/>
-    <mergeCell ref="BM3:BT3"/>
-    <mergeCell ref="BL2:BU2"/>
-    <mergeCell ref="AO5:AS5"/>
-    <mergeCell ref="AL4:AS4"/>
-    <mergeCell ref="AI3:AT3"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="BA5:BE5"/>
-    <mergeCell ref="AX4:BE4"/>
-    <mergeCell ref="AU3:BF3"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AG5"/>
-    <mergeCell ref="Z4:AG4"/>
-    <mergeCell ref="W3:AH3"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:T5"/>
-    <mergeCell ref="M4:T4"/>
-    <mergeCell ref="I3:T3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C1000001 CU8:CU1000001 CQ8:CQ1000001 BU8:BU1000001 BL8:BL1000001 BJ8:BJ1000001 BF8:BF1000001 AT8:AT1000001 AH8:AH1000001" xr:uid="{00000000-0002-0000-0100-000001000000}">
@@ -42366,21 +42369,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="F2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="W2:AE2"/>
+    <mergeCell ref="AF3:AK3"/>
+    <mergeCell ref="AL3:AR3"/>
+    <mergeCell ref="AF2:AR2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AU2:AW2"/>
     <mergeCell ref="AY3:BC3"/>
     <mergeCell ref="AX2:BD2"/>
     <mergeCell ref="BH3:BI3"/>
     <mergeCell ref="BN3:BO3"/>
     <mergeCell ref="BG2:BO2"/>
-    <mergeCell ref="AF3:AK3"/>
-    <mergeCell ref="AL3:AR3"/>
-    <mergeCell ref="AF2:AR2"/>
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AU2:AW2"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="F2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="W2:AE2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E1000001 BH6:BH1000001 BD6:BD1000001 T6:T1000001" xr:uid="{00000000-0002-0000-0200-000002000000}">
@@ -45694,6 +45697,58 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="H3:N3"/>
+    <mergeCell ref="D2:N2"/>
+    <mergeCell ref="V4:Z4"/>
+    <mergeCell ref="BI4:BM4"/>
+    <mergeCell ref="BS5:BW5"/>
+    <mergeCell ref="BR4:BX4"/>
+    <mergeCell ref="BB3:BX3"/>
+    <mergeCell ref="O2:BX2"/>
+    <mergeCell ref="AF5:AJ5"/>
+    <mergeCell ref="AE4:AK4"/>
+    <mergeCell ref="O3:AK3"/>
+    <mergeCell ref="AO4:AS4"/>
+    <mergeCell ref="AV5:AZ5"/>
+    <mergeCell ref="AU4:BA4"/>
+    <mergeCell ref="AL3:BA3"/>
+    <mergeCell ref="BY2:CB2"/>
+    <mergeCell ref="CD3:CE3"/>
+    <mergeCell ref="CH6:CI6"/>
+    <mergeCell ref="CJ6:CN6"/>
+    <mergeCell ref="CG5:CN5"/>
+    <mergeCell ref="CO5:CS5"/>
+    <mergeCell ref="CG4:CS4"/>
+    <mergeCell ref="CG3:CU3"/>
+    <mergeCell ref="CW6:CX6"/>
+    <mergeCell ref="CY6:DC6"/>
+    <mergeCell ref="CV5:DC5"/>
+    <mergeCell ref="DD5:DH5"/>
+    <mergeCell ref="CV4:DH4"/>
+    <mergeCell ref="CV3:DJ3"/>
+    <mergeCell ref="DL4:DP4"/>
+    <mergeCell ref="DK3:DQ3"/>
+    <mergeCell ref="DS4:DT4"/>
+    <mergeCell ref="DY4:DZ4"/>
+    <mergeCell ref="DR3:DZ3"/>
+    <mergeCell ref="EF7:EG7"/>
+    <mergeCell ref="EH7:EI7"/>
+    <mergeCell ref="EJ7:EM7"/>
+    <mergeCell ref="EF6:EM6"/>
+    <mergeCell ref="ED5:EO5"/>
+    <mergeCell ref="EB4:EO4"/>
+    <mergeCell ref="EP4:EQ4"/>
+    <mergeCell ref="FR4:FU4"/>
+    <mergeCell ref="FV4:FX4"/>
+    <mergeCell ref="FZ5:GD5"/>
+    <mergeCell ref="FY4:GE4"/>
+    <mergeCell ref="FC5:FD5"/>
+    <mergeCell ref="FE5:FI5"/>
+    <mergeCell ref="FB4:FI4"/>
+    <mergeCell ref="FK5:FL5"/>
+    <mergeCell ref="FJ4:FM4"/>
     <mergeCell ref="GW3:HK3"/>
     <mergeCell ref="HL3:HM3"/>
     <mergeCell ref="CC2:HN2"/>
@@ -45710,58 +45765,6 @@
     <mergeCell ref="EA3:GS3"/>
     <mergeCell ref="FN4:FQ4"/>
     <mergeCell ref="FS5:FT5"/>
-    <mergeCell ref="FR4:FU4"/>
-    <mergeCell ref="FV4:FX4"/>
-    <mergeCell ref="FZ5:GD5"/>
-    <mergeCell ref="FY4:GE4"/>
-    <mergeCell ref="FC5:FD5"/>
-    <mergeCell ref="FE5:FI5"/>
-    <mergeCell ref="FB4:FI4"/>
-    <mergeCell ref="FK5:FL5"/>
-    <mergeCell ref="FJ4:FM4"/>
-    <mergeCell ref="EJ7:EM7"/>
-    <mergeCell ref="EF6:EM6"/>
-    <mergeCell ref="ED5:EO5"/>
-    <mergeCell ref="EB4:EO4"/>
-    <mergeCell ref="EP4:EQ4"/>
-    <mergeCell ref="DS4:DT4"/>
-    <mergeCell ref="DY4:DZ4"/>
-    <mergeCell ref="DR3:DZ3"/>
-    <mergeCell ref="EF7:EG7"/>
-    <mergeCell ref="EH7:EI7"/>
-    <mergeCell ref="DD5:DH5"/>
-    <mergeCell ref="CV4:DH4"/>
-    <mergeCell ref="CV3:DJ3"/>
-    <mergeCell ref="DL4:DP4"/>
-    <mergeCell ref="DK3:DQ3"/>
-    <mergeCell ref="CO5:CS5"/>
-    <mergeCell ref="CG4:CS4"/>
-    <mergeCell ref="CG3:CU3"/>
-    <mergeCell ref="CW6:CX6"/>
-    <mergeCell ref="CY6:DC6"/>
-    <mergeCell ref="CV5:DC5"/>
-    <mergeCell ref="BY2:CB2"/>
-    <mergeCell ref="CD3:CE3"/>
-    <mergeCell ref="CH6:CI6"/>
-    <mergeCell ref="CJ6:CN6"/>
-    <mergeCell ref="CG5:CN5"/>
-    <mergeCell ref="BI4:BM4"/>
-    <mergeCell ref="BS5:BW5"/>
-    <mergeCell ref="BR4:BX4"/>
-    <mergeCell ref="BB3:BX3"/>
-    <mergeCell ref="O2:BX2"/>
-    <mergeCell ref="AF5:AJ5"/>
-    <mergeCell ref="AE4:AK4"/>
-    <mergeCell ref="O3:AK3"/>
-    <mergeCell ref="AO4:AS4"/>
-    <mergeCell ref="AV5:AZ5"/>
-    <mergeCell ref="AU4:BA4"/>
-    <mergeCell ref="AL3:BA3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="I4:M4"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="D2:N2"/>
-    <mergeCell ref="V4:Z4"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D1000001 HO10:HP1000001 HJ10:HJ1000001 GG10:GG1000001 GE10:GE1000001 FX10:FX1000001 EX10:EY1000001 DS10:DS1000001 DQ10:DQ1000001 DI10:DI1000001 CT10:CT1000001 BX10:BX1000001 BA10:BB1000001 AK10:AL1000001 N10:O1000001" xr:uid="{00000000-0002-0000-0300-000001000000}">
@@ -46673,23 +46676,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:AB3"/>
+    <mergeCell ref="U2:AB2"/>
+    <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AH2:AJ2"/>
     <mergeCell ref="AM3:AQ3"/>
     <mergeCell ref="AL2:AR2"/>
     <mergeCell ref="AT3:AU3"/>
     <mergeCell ref="AZ3:BA3"/>
     <mergeCell ref="AS2:BA2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:AB3"/>
-    <mergeCell ref="U2:AB2"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="J2:Q2"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT6:AT1000001 AR6:AR1000001 AC6:AD1000001" xr:uid="{00000000-0002-0000-0400-000000000000}">

</xml_diff>